<commit_message>
Commit Siebel Service updates
</commit_message>
<xml_diff>
--- a/Dev/Files/Siebel Service/ITAF_DataBank_Service_MSPatch.xlsx
+++ b/Dev/Files/Siebel Service/ITAF_DataBank_Service_MSPatch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="169">
   <si>
     <t>TC_ID</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>1-G9MHVB</t>
+  </si>
+  <si>
+    <t>MS Patching 15Feb2019 Please Ignore</t>
   </si>
 </sst>
 </file>
@@ -1397,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,7 +1584,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:56" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>62</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>55</v>
@@ -1631,7 +1634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:56" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>62</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>55</v>
@@ -1681,7 +1684,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:56" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:56" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>73</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>162</v>
@@ -1731,7 +1734,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:56" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:56" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>74</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>166</v>

</xml_diff>